<commit_message>
Create Generation 4M of the models
1.  Build the following models for each dataset/partition:
  Plain TN
  TN/RGBOOST (MHESS=0)
  TN/RGBOOST (MHESS=1)
  XGBoost

2.  Expand all categorical predictors into sets of dummies.

3.  Create more detailed summary report

Also, fix bug in sumrept4.py (one set of models from each dataset were being ignored.
</commit_message>
<xml_diff>
--- a/Reports/tn_vs_xgb_sumrept4.xlsx
+++ b/Reports/tn_vs_xgb_sumrept4.xlsx
@@ -222,20 +222,20 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,16 +293,16 @@
         <v>50</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0.867395762132604</v>
+        <v>0.870373376623376</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.847787081339713</v>
+        <v>0.852069805194805</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>0.0644486031385768</v>
+        <v>0.0641274863059178</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0.0196086807928913</v>
+        <v>0.0183035714285714</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>-0.0357142857142857</v>
@@ -311,7 +311,7 @@
         <v>0.0633116883116883</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>0.030016940476815</v>
+        <v>0.0297936401308394</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,25 +331,25 @@
         <v>12210</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0.926650577612171</v>
+        <v>0.926607638944159</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.927369476378435</v>
+        <v>0.927269238317118</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0.00142739382751065</v>
+        <v>0.00140253105038784</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>-0.000718898766263661</v>
+        <v>-0.00066159937295906</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>-0.00218585166673446</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0.000376130233029737</v>
+        <v>0.000427089099828359</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>0.000637812011529779</v>
+        <v>0.000671608387486361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,16 +369,16 @@
         <v>1750</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.99665519226638</v>
+        <v>0.99659787755102</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.996410191192267</v>
+        <v>0.996371689795919</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0.00108714962626378</v>
+        <v>0.00108875565584885</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.000245001074113878</v>
+        <v>0.000226187755102064</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>-0.000372897959183716</v>
@@ -387,7 +387,7 @@
         <v>0.00101159183673472</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>0.000346469633817808</v>
+        <v>0.000347565919404055</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,25 +407,25 @@
         <v>650</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.86817116163189</v>
+        <v>0.867891124260355</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.860409841170975</v>
+        <v>0.861014437869823</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.0324826874837014</v>
+        <v>0.0316411205671404</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.00776132046091561</v>
+        <v>0.00687668639053254</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>-0.00964733727810663</v>
+        <v>-0.00993136094674563</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>0.0289704142011835</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0.0110013843256464</v>
+        <v>0.011415427359208</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,16 +445,16 @@
         <v>4755</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.931368169921192</v>
+        <v>0.931552243977236</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.930970541738993</v>
+        <v>0.93109162260397</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>0.00279707851610416</v>
+        <v>0.00284421209268822</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.000397628182199607</v>
+        <v>0.000460621373266234</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>-0.00232871418661063</v>
@@ -463,7 +463,7 @@
         <v>0.00363323255947501</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0.00148114571983926</v>
+        <v>0.00146890868167771</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,16 +483,16 @@
         <v>1850</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.996861276813964</v>
+        <v>0.996868133024134</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.997251856252002</v>
+        <v>0.997243858878094</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.000681100375984766</v>
+        <v>0.000663643130708652</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>-0.000390579438038073</v>
+        <v>-0.000375725853959585</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>-0.00103209186201991</v>
@@ -501,7 +501,7 @@
         <v>5.72735008368408E-005</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0.000307140041565986</v>
+        <v>0.000306239422776564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,16 +521,16 @@
         <v>1150</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.987081266974481</v>
+        <v>0.987197497315838</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.986599609706757</v>
+        <v>0.986778087103037</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0.00205597680312486</v>
+        <v>0.00206754797723952</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>0.000481657267723932</v>
+        <v>0.000419410212801008</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>-0.00101032175105553</v>
@@ -539,7 +539,7 @@
         <v>0.00174826835919317</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>0.000726758689692923</v>
+        <v>0.000760179753551909</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,16 +559,16 @@
         <v>1850</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.995683087924339</v>
+        <v>0.995629306062819</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.995286055899427</v>
+        <v>0.995234360847334</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0.000634240367815726</v>
+        <v>0.000662524711509844</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>0.000397032024912545</v>
+        <v>0.000394945215485765</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>-0.000199853907962067</v>
@@ -577,7 +577,7 @@
         <v>0.00127158509861225</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0.000415967715637934</v>
+        <v>0.000404980788505783</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,25 +597,25 @@
         <v>172</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.916073677015505</v>
+        <v>0.913113465481886</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.912102025398424</v>
+        <v>0.908465481886534</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.0180931239775592</v>
+        <v>0.0220315375838272</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0.00397165161708099</v>
+        <v>0.00464798359535203</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>-0.00991114149008887</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0.0170881749829118</v>
+        <v>0.0174982911825017</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0.00777986971331811</v>
+        <v>0.00815409547937284</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,16 +635,16 @@
         <v>76</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.681672932330827</v>
+        <v>0.683147321428572</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.649130639097744</v>
+        <v>0.652276785714286</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.0595172008392728</v>
+        <v>0.0583038331969737</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>0.0325422932330827</v>
+        <v>0.0308705357142857</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>-0.025</v>
@@ -653,7 +653,7 @@
         <v>0.138392857142857</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>0.0426112361533678</v>
+        <v>0.0421431944021646</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,16 +673,16 @@
         <v>819</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.972099762283649</v>
+        <v>0.972452718676123</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.974479545261062</v>
+        <v>0.974599041931069</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.0119417806207309</v>
+        <v>0.0117299660357151</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>-0.0023797829774137</v>
+        <v>-0.00214632325494591</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>-0.0112479781012816</v>
@@ -691,7 +691,7 @@
         <v>0.00660072166231174</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>0.00479582408754742</v>
+        <v>0.0047832494140446</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,16 +711,16 @@
         <v>1649</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.997456727077197</v>
+        <v>0.99752730505461</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.996429956017807</v>
+        <v>0.996505870233963</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.00138285486063737</v>
+        <v>0.00138248539577278</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0.00102677105939008</v>
+        <v>0.00102143482064743</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>-0.000850901701803464</v>
@@ -729,7 +729,7 @@
         <v>0.00266841644794391</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>0.000841118237697587</v>
+        <v>0.000819032120855366</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,16 +749,16 @@
         <v>11302</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.931991896046253</v>
+        <v>0.932140764130379</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.93158201106409</v>
+        <v>0.931772463232062</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.00265756116646092</v>
+        <v>0.0026709825988296</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>0.000409884982162796</v>
+        <v>0.000368300898317103</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>-0.00102345386688652</v>
@@ -767,7 +767,7 @@
         <v>0.00212986487346867</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0.00103888342783283</v>
+        <v>0.00102813391689663</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,16 +787,16 @@
         <v>646</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.709038447095408</v>
+        <v>0.710342666512399</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.684148616363308</v>
+        <v>0.686652975432913</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0.0418300256368105</v>
+        <v>0.0411300212773829</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>0.0248898307321004</v>
+        <v>0.0236896910794863</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>-0.0376605345366192</v>
@@ -805,7 +805,7 @@
         <v>0.087913147441089</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0.0351850422956926</v>
+        <v>0.0346646315996801</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,16 +825,16 @@
         <v>825</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.751897373109494</v>
+        <v>0.752220117845118</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0.731714974139217</v>
+        <v>0.731378175696357</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.045061246796585</v>
+        <v>0.0445265989894734</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>0.0201823989702777</v>
+        <v>0.0208419421487603</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>-0.0430058157330884</v>
@@ -843,7 +843,7 @@
         <v>0.103611876339149</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0.0334750146635667</v>
+        <v>0.0333053113090319</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,16 +863,16 @@
         <v>3796</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.849870257822824</v>
+        <v>0.850284430030089</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.83921530321636</v>
+        <v>0.839103117446851</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>0.0154547155118348</v>
+        <v>0.0151561223385738</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>0.0106549546064639</v>
+        <v>0.0111813125832388</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>-0.0026957036452423</v>
@@ -881,7 +881,7 @@
         <v>0.0278868445715976</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>0.00919982431133716</v>
+        <v>0.00925868538457982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>